<commit_message>
Updated forest reserve guidance.
</commit_message>
<xml_diff>
--- a/docs/lux-backend-sizing.xlsx
+++ b/docs/lux-backend-sizing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\repos\marklogic\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25925663-4DF8-4BA9-92CD-8437D62B94CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BA54A2-07F8-4B3D-B91C-11D73F7A3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group-Level Caches" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="149">
   <si>
     <t>DEV</t>
   </si>
@@ -413,12 +413,6 @@
     <t>Size required by forests per volume:</t>
   </si>
   <si>
-    <t>Beta 1 dataset and Backend v1.0.8 database indexing configuration</t>
-  </si>
-  <si>
-    <t>2 * MIN(forest size, maximum merge size)</t>
-  </si>
-  <si>
     <t>Beta 2 WIP at commit https://git.yale.edu/LUX/pipeline/commit/8bf569847f9304211ecdabc8bdc6b5164eedb24f</t>
   </si>
   <si>
@@ -428,12 +422,6 @@
     <t>Per admin UI.  Primary forests only.  Excludes journals.</t>
   </si>
   <si>
-    <t>23 Jan 23 DEV with Beta 2 (final) dataset and Backend v1.0.10 WIP (no index changes)</t>
-  </si>
-  <si>
-    <t>3 Mar 23 SBX before enabling word positions (#635 experiment)</t>
-  </si>
-  <si>
     <t>Beta 2's indexing configuration.</t>
   </si>
   <si>
@@ -453,6 +441,51 @@
   </si>
   <si>
     <t>Ticket #920 summary: TODO</t>
+  </si>
+  <si>
+    <t>Replicated Once</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4 GB per forest</t>
+  </si>
+  <si>
+    <t>30 days of logs</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Primary forests</t>
+  </si>
+  <si>
+    <t>Replicated forest</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>1.5x forest size</t>
+  </si>
+  <si>
+    <t>2x merge max</t>
+  </si>
+  <si>
+    <t>Scenario 1 with the 2024-12-14 dataset</t>
+  </si>
+  <si>
+    <t>Scenario 2 with the 2024-12-14 dataset</t>
+  </si>
+  <si>
+    <t>Pasted into lux-backend-infrastructure.md</t>
+  </si>
+  <si>
+    <t>Not Replicated</t>
   </si>
 </sst>
 </file>
@@ -465,7 +498,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,6 +561,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -607,7 +648,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -719,21 +760,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -755,6 +806,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -787,6 +839,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
@@ -1216,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555E99A3-6377-4031-9CA1-0E245380646D}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1255,7 +1308,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -1285,14 +1338,14 @@
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
@@ -1317,14 +1370,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="22"/>
@@ -1479,14 +1532,14 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
@@ -1507,14 +1560,14 @@
       <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
     </row>
     <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
@@ -1536,14 +1589,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="27" t="s">
@@ -1564,11 +1617,11 @@
       <c r="H20" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="18.45" x14ac:dyDescent="0.4">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="22"/>
@@ -1636,11 +1689,11 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.45" x14ac:dyDescent="0.4">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="22"/>
@@ -1789,134 +1842,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="3">
         <v>44936</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="51"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="3">
         <v>44957</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="51"/>
+      <c r="L2" s="55"/>
       <c r="M2" s="3">
         <v>44988</v>
       </c>
       <c r="N2" s="2"/>
-      <c r="P2" s="51" t="s">
+      <c r="P2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="51"/>
+      <c r="Q2" s="55"/>
       <c r="R2" s="3">
         <v>45063</v>
       </c>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="51"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="51"/>
+      <c r="L3" s="55"/>
       <c r="M3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="P3" s="51" t="s">
+      <c r="P3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="51"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="51"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="K4" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" s="55"/>
+      <c r="M4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="K4" s="51" t="s">
+      <c r="N4" s="2"/>
+      <c r="P4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="2" t="s">
+      <c r="Q4" s="55"/>
+      <c r="R4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="P4" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="51"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="51"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="K5" s="51" t="s">
+      <c r="K5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="51"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="P5" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="P5" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="S5" s="2"/>
     </row>
@@ -2595,10 +2648,10 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="36">
         <f>B19+C19</f>
         <v>59913</v>
@@ -2606,10 +2659,10 @@
       <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="50"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="36">
         <f>G19+H19</f>
         <v>45441</v>
@@ -2617,10 +2670,10 @@
       <c r="I20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="54"/>
       <c r="M20" s="36">
         <f>L19+M19</f>
         <v>52425</v>
@@ -2628,10 +2681,10 @@
       <c r="N20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P20" s="50" t="s">
+      <c r="P20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="50"/>
+      <c r="Q20" s="54"/>
       <c r="R20" s="36">
         <f>Q19+R19</f>
         <v>51642</v>
@@ -2641,8 +2694,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="38">
         <f>C20/1024</f>
         <v>58.5087890625</v>
@@ -2650,8 +2703,8 @@
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="38">
         <f>H20/1024</f>
         <v>44.3759765625</v>
@@ -2659,8 +2712,8 @@
       <c r="I21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
       <c r="M21" s="38">
         <f>M20/1024</f>
         <v>51.1962890625</v>
@@ -2668,8 +2721,8 @@
       <c r="N21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
       <c r="R21" s="38">
         <f>R20/1024</f>
         <v>50.431640625</v>
@@ -2679,10 +2732,10 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="40">
         <f>C20/3</f>
         <v>19971</v>
@@ -2690,10 +2743,10 @@
       <c r="D22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="50"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="36">
         <f>H20/3</f>
         <v>15147</v>
@@ -2701,10 +2754,10 @@
       <c r="I22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="50" t="s">
+      <c r="K22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="L22" s="50"/>
+      <c r="L22" s="54"/>
       <c r="M22" s="36">
         <f>M20/3</f>
         <v>17475</v>
@@ -2712,10 +2765,10 @@
       <c r="N22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P22" s="50" t="s">
+      <c r="P22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="Q22" s="50"/>
+      <c r="Q22" s="54"/>
       <c r="R22" s="36">
         <f>R20/3</f>
         <v>17214</v>
@@ -2725,8 +2778,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="38">
         <f>C21/3</f>
         <v>19.5029296875</v>
@@ -2734,8 +2787,8 @@
       <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="38">
         <f>H21/3</f>
         <v>14.7919921875</v>
@@ -2743,8 +2796,8 @@
       <c r="I23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
       <c r="M23" s="38">
         <f>M21/3</f>
         <v>17.0654296875</v>
@@ -2752,8 +2805,8 @@
       <c r="N23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
       <c r="R23" s="38">
         <f>R21/3</f>
         <v>16.810546875</v>
@@ -2764,30 +2817,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K22:L23"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K20:L21"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F20:G21"/>
     <mergeCell ref="P22:Q23"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="P20:Q21"/>
-    <mergeCell ref="F22:G23"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K22:L23"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K20:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2918,19 +2971,19 @@
       <c r="B13" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="G15" s="52" t="s">
+      <c r="E15" s="56"/>
+      <c r="G15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
@@ -3107,16 +3160,16 @@
       <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
@@ -3132,14 +3185,14 @@
       <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3517,445 +3570,494 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="37.84375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="12.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.84375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="42" customWidth="1"/>
     <col min="3" max="3" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.84375" style="42" customWidth="1"/>
-    <col min="5" max="5" width="12.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.765625" style="42" customWidth="1"/>
+    <col min="5" max="5" width="12.84375" style="42" customWidth="1"/>
     <col min="6" max="6" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.84375" style="42" customWidth="1"/>
-    <col min="9" max="9" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.765625" style="42" customWidth="1"/>
-    <col min="11" max="11" width="4.69140625" style="42" customWidth="1"/>
-    <col min="12" max="12" width="18.4609375" style="42" customWidth="1"/>
-    <col min="13" max="16384" width="9.23046875" style="10"/>
+    <col min="7" max="7" width="12.765625" style="42" customWidth="1"/>
+    <col min="8" max="8" width="4.69140625" style="42" customWidth="1"/>
+    <col min="9" max="9" width="18.4609375" style="42" customWidth="1"/>
+    <col min="10" max="13" width="9.23046875" style="10"/>
+    <col min="14" max="14" width="14.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.61328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.3828125" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.23046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.3828125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.23046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.23046875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:19" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="44" t="s">
+      <c r="B1" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A2" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="10">
-        <v>777</v>
+      <c r="B2" s="45">
+        <v>630</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12">
-        <f>521057/1024</f>
-        <v>508.8447265625</v>
+      <c r="E2" s="45">
+        <v>630</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12">
-        <f>525842/1024</f>
-        <v>513.517578125</v>
-      </c>
       <c r="I2" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A3" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="45">
         <v>9</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="45">
         <v>9</v>
       </c>
-      <c r="H3" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="44" t="s">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="45">
         <f>B2/B3</f>
-        <v>86.333333333333329</v>
+        <v>70</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="45">
         <f>E2/E3</f>
-        <v>56.538302951388886</v>
+        <v>70</v>
       </c>
       <c r="F4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12">
-        <f>H2/H3</f>
-        <v>57.057508680555557</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="44" t="s">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="45">
         <v>48</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="45">
         <v>48</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="10">
-        <v>48</v>
-      </c>
       <c r="I5" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A6" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="10">
-        <f>MIN(B4, B5)*2</f>
-        <v>96</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="B6" s="49">
+        <f>B4*1.5</f>
+        <v>105</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="49">
         <f>MIN(E4, E5)*2</f>
         <v>96</v>
       </c>
-      <c r="F6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="10">
-        <f>MIN(H4, H5)*2</f>
-        <v>96</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="44" t="s">
+      <c r="F6" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B7" s="45"/>
+      <c r="E7" s="45"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="45">
+        <v>0</v>
+      </c>
+      <c r="E8" s="45">
+        <v>0</v>
+      </c>
+      <c r="N8" s="50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="45">
+        <v>3</v>
+      </c>
+      <c r="E9" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E10" s="45">
         <v>1</v>
       </c>
-      <c r="H8" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="10">
-        <v>3</v>
-      </c>
-      <c r="E9" s="10">
-        <v>3</v>
-      </c>
-      <c r="H9" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="44" t="s">
+      <c r="N10" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="O10" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" s="51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="N11" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="O11" s="51">
+        <f>B2/B3*3</f>
+        <v>210</v>
+      </c>
+      <c r="P11" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="51">
+        <f>O11</f>
+        <v>210</v>
+      </c>
+      <c r="R11" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A12" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="45">
         <f>B6*B3</f>
-        <v>864</v>
+        <v>945</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="45">
         <f>E6*E3</f>
         <v>864</v>
       </c>
       <c r="F12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="10">
-        <f>H6*H3</f>
+      <c r="N12" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="O12" s="51">
+        <v>0</v>
+      </c>
+      <c r="P12" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="51">
+        <f>Q11</f>
+        <v>210</v>
+      </c>
+      <c r="R12" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S12" s="51"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="45">
+        <f>B12*B8</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="45">
+        <f>E12*E8</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="51">
+        <f>1.5*O11</f>
+        <v>315</v>
+      </c>
+      <c r="P13" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="51">
+        <f>1.5*(Q11+Q12)</f>
+        <v>630</v>
+      </c>
+      <c r="R13" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A14" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="46">
+        <f>B12+B13</f>
+        <v>945</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="46">
+        <f>E12+E13</f>
         <v>864</v>
       </c>
-      <c r="I12" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A13" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="10">
-        <f>B12*B8</f>
-        <v>864</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="10">
-        <f>E12*E8</f>
-        <v>864</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="10">
-        <f>H12*H8</f>
-        <v>864</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="43">
-        <f>B12+B13</f>
-        <v>1728</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="43">
-        <f>E12+E13</f>
-        <v>1728</v>
-      </c>
       <c r="F14" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="43">
-        <f>H12+H13</f>
-        <v>1728</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" s="44" t="s">
+      <c r="N14" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="51">
+        <f>4*3</f>
+        <v>12</v>
+      </c>
+      <c r="P14" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="51">
+        <f>4*6</f>
+        <v>24</v>
+      </c>
+      <c r="R14" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" s="51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="N15" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="51">
+        <v>2</v>
+      </c>
+      <c r="P15" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>2</v>
+      </c>
+      <c r="R15" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A16" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="45">
         <f>B2/B9/B10</f>
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="45">
         <f>E2/E9/E10</f>
-        <v>169.61490885416666</v>
+        <v>210</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="12">
-        <f>H2/H9/H10</f>
-        <v>171.17252604166666</v>
-      </c>
-      <c r="I16" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="44" t="s">
+      <c r="N16" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="O16" s="59">
+        <f>SUM(O11:O15)</f>
+        <v>539</v>
+      </c>
+      <c r="P16" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="59">
+        <f>SUM(Q11:Q15)</f>
+        <v>1076</v>
+      </c>
+      <c r="R16" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="S16" s="59" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="45">
         <f>B16*B8</f>
-        <v>259</v>
+        <v>0</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="45">
         <f>E16*E8</f>
-        <v>169.61490885416666</v>
+        <v>0</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="12">
-        <f>H16*H8</f>
-        <v>171.17252604166666</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="44" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="45">
         <f>B12/B9/B10</f>
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="C18" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="45">
         <f>E12/E9/E10</f>
         <v>288</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="12">
-        <f>H12/H9/H10</f>
-        <v>288</v>
-      </c>
-      <c r="I18" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="44" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="45">
         <f>B18*B8</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="45">
         <f>E18*E8</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="12">
-        <f>H18*H8</f>
-        <v>288</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="44" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="46">
         <f>SUM(B16:B19)</f>
-        <v>1094</v>
+        <v>525</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="46">
         <f>SUM(E16:E19)</f>
-        <v>915.22981770833326</v>
+        <v>498</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="45">
-        <f>SUM(H16:H19)</f>
-        <v>918.34505208333326</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="47">
-        <v>40806746</v>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="44">
+        <f>42063754</f>
+        <v>42063754</v>
+      </c>
+      <c r="E24" s="44">
+        <f>B24</f>
+        <v>42063754</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated forest reserve guidance. (#405)
</commit_message>
<xml_diff>
--- a/docs/lux-backend-sizing.xlsx
+++ b/docs/lux-backend-sizing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\repos\marklogic\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25925663-4DF8-4BA9-92CD-8437D62B94CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BA54A2-07F8-4B3D-B91C-11D73F7A3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group-Level Caches" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="149">
   <si>
     <t>DEV</t>
   </si>
@@ -413,12 +413,6 @@
     <t>Size required by forests per volume:</t>
   </si>
   <si>
-    <t>Beta 1 dataset and Backend v1.0.8 database indexing configuration</t>
-  </si>
-  <si>
-    <t>2 * MIN(forest size, maximum merge size)</t>
-  </si>
-  <si>
     <t>Beta 2 WIP at commit https://git.yale.edu/LUX/pipeline/commit/8bf569847f9304211ecdabc8bdc6b5164eedb24f</t>
   </si>
   <si>
@@ -428,12 +422,6 @@
     <t>Per admin UI.  Primary forests only.  Excludes journals.</t>
   </si>
   <si>
-    <t>23 Jan 23 DEV with Beta 2 (final) dataset and Backend v1.0.10 WIP (no index changes)</t>
-  </si>
-  <si>
-    <t>3 Mar 23 SBX before enabling word positions (#635 experiment)</t>
-  </si>
-  <si>
     <t>Beta 2's indexing configuration.</t>
   </si>
   <si>
@@ -453,6 +441,51 @@
   </si>
   <si>
     <t>Ticket #920 summary: TODO</t>
+  </si>
+  <si>
+    <t>Replicated Once</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4 GB per forest</t>
+  </si>
+  <si>
+    <t>30 days of logs</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Primary forests</t>
+  </si>
+  <si>
+    <t>Replicated forest</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>1.5x forest size</t>
+  </si>
+  <si>
+    <t>2x merge max</t>
+  </si>
+  <si>
+    <t>Scenario 1 with the 2024-12-14 dataset</t>
+  </si>
+  <si>
+    <t>Scenario 2 with the 2024-12-14 dataset</t>
+  </si>
+  <si>
+    <t>Pasted into lux-backend-infrastructure.md</t>
+  </si>
+  <si>
+    <t>Not Replicated</t>
   </si>
 </sst>
 </file>
@@ -465,7 +498,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,6 +561,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -607,7 +648,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -719,21 +760,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -755,6 +806,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -787,6 +839,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
@@ -1216,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555E99A3-6377-4031-9CA1-0E245380646D}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1255,7 +1308,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -1285,14 +1338,14 @@
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
@@ -1317,14 +1370,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="22"/>
@@ -1479,14 +1532,14 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
@@ -1507,14 +1560,14 @@
       <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
     </row>
     <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
@@ -1536,14 +1589,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="27" t="s">
@@ -1564,11 +1617,11 @@
       <c r="H20" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="18.45" x14ac:dyDescent="0.4">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="22"/>
@@ -1636,11 +1689,11 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.45" x14ac:dyDescent="0.4">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="22"/>
@@ -1789,134 +1842,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="3">
         <v>44936</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="51"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="3">
         <v>44957</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="51"/>
+      <c r="L2" s="55"/>
       <c r="M2" s="3">
         <v>44988</v>
       </c>
       <c r="N2" s="2"/>
-      <c r="P2" s="51" t="s">
+      <c r="P2" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="51"/>
+      <c r="Q2" s="55"/>
       <c r="R2" s="3">
         <v>45063</v>
       </c>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="51"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="51"/>
+      <c r="L3" s="55"/>
       <c r="M3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="P3" s="51" t="s">
+      <c r="P3" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="51"/>
+      <c r="Q3" s="55"/>
       <c r="R3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="51"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="K4" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" s="55"/>
+      <c r="M4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="K4" s="51" t="s">
+      <c r="N4" s="2"/>
+      <c r="P4" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="2" t="s">
+      <c r="Q4" s="55"/>
+      <c r="R4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="P4" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="51"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="51"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="K5" s="51" t="s">
+      <c r="K5" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="51"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="P5" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="P5" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="S5" s="2"/>
     </row>
@@ -2595,10 +2648,10 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="36">
         <f>B19+C19</f>
         <v>59913</v>
@@ -2606,10 +2659,10 @@
       <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="50"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="36">
         <f>G19+H19</f>
         <v>45441</v>
@@ -2617,10 +2670,10 @@
       <c r="I20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="54"/>
       <c r="M20" s="36">
         <f>L19+M19</f>
         <v>52425</v>
@@ -2628,10 +2681,10 @@
       <c r="N20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P20" s="50" t="s">
+      <c r="P20" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="50"/>
+      <c r="Q20" s="54"/>
       <c r="R20" s="36">
         <f>Q19+R19</f>
         <v>51642</v>
@@ -2641,8 +2694,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="38">
         <f>C20/1024</f>
         <v>58.5087890625</v>
@@ -2650,8 +2703,8 @@
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="38">
         <f>H20/1024</f>
         <v>44.3759765625</v>
@@ -2659,8 +2712,8 @@
       <c r="I21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
       <c r="M21" s="38">
         <f>M20/1024</f>
         <v>51.1962890625</v>
@@ -2668,8 +2721,8 @@
       <c r="N21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
       <c r="R21" s="38">
         <f>R20/1024</f>
         <v>50.431640625</v>
@@ -2679,10 +2732,10 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="40">
         <f>C20/3</f>
         <v>19971</v>
@@ -2690,10 +2743,10 @@
       <c r="D22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="50"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="36">
         <f>H20/3</f>
         <v>15147</v>
@@ -2701,10 +2754,10 @@
       <c r="I22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="50" t="s">
+      <c r="K22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="L22" s="50"/>
+      <c r="L22" s="54"/>
       <c r="M22" s="36">
         <f>M20/3</f>
         <v>17475</v>
@@ -2712,10 +2765,10 @@
       <c r="N22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P22" s="50" t="s">
+      <c r="P22" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="Q22" s="50"/>
+      <c r="Q22" s="54"/>
       <c r="R22" s="36">
         <f>R20/3</f>
         <v>17214</v>
@@ -2725,8 +2778,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="38">
         <f>C21/3</f>
         <v>19.5029296875</v>
@@ -2734,8 +2787,8 @@
       <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="38">
         <f>H21/3</f>
         <v>14.7919921875</v>
@@ -2743,8 +2796,8 @@
       <c r="I23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
       <c r="M23" s="38">
         <f>M21/3</f>
         <v>17.0654296875</v>
@@ -2752,8 +2805,8 @@
       <c r="N23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
       <c r="R23" s="38">
         <f>R21/3</f>
         <v>16.810546875</v>
@@ -2764,30 +2817,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K22:L23"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K20:L21"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F20:G21"/>
     <mergeCell ref="P22:Q23"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="P20:Q21"/>
-    <mergeCell ref="F22:G23"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K22:L23"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K20:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2918,19 +2971,19 @@
       <c r="B13" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="G15" s="52" t="s">
+      <c r="E15" s="56"/>
+      <c r="G15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
@@ -3107,16 +3160,16 @@
       <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
@@ -3132,14 +3185,14 @@
       <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3517,445 +3570,494 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="37.84375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="12.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.84375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" style="42" customWidth="1"/>
     <col min="3" max="3" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.84375" style="42" customWidth="1"/>
-    <col min="5" max="5" width="12.15234375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.765625" style="42" customWidth="1"/>
+    <col min="5" max="5" width="12.84375" style="42" customWidth="1"/>
     <col min="6" max="6" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.84375" style="42" customWidth="1"/>
-    <col min="9" max="9" width="4.69140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.765625" style="42" customWidth="1"/>
-    <col min="11" max="11" width="4.69140625" style="42" customWidth="1"/>
-    <col min="12" max="12" width="18.4609375" style="42" customWidth="1"/>
-    <col min="13" max="16384" width="9.23046875" style="10"/>
+    <col min="7" max="7" width="12.765625" style="42" customWidth="1"/>
+    <col min="8" max="8" width="4.69140625" style="42" customWidth="1"/>
+    <col min="9" max="9" width="18.4609375" style="42" customWidth="1"/>
+    <col min="10" max="13" width="9.23046875" style="10"/>
+    <col min="14" max="14" width="14.84375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.61328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.3828125" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.23046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.3828125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.23046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.23046875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:19" ht="44.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="44" t="s">
+      <c r="B1" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A2" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="10">
-        <v>777</v>
+      <c r="B2" s="45">
+        <v>630</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12">
-        <f>521057/1024</f>
-        <v>508.8447265625</v>
+      <c r="E2" s="45">
+        <v>630</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12">
-        <f>525842/1024</f>
-        <v>513.517578125</v>
-      </c>
       <c r="I2" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A3" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="45">
         <v>9</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="45">
         <v>9</v>
       </c>
-      <c r="H3" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="44" t="s">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="45">
         <f>B2/B3</f>
-        <v>86.333333333333329</v>
+        <v>70</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="45">
         <f>E2/E3</f>
-        <v>56.538302951388886</v>
+        <v>70</v>
       </c>
       <c r="F4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12">
-        <f>H2/H3</f>
-        <v>57.057508680555557</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="44" t="s">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="45">
         <v>48</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="45">
         <v>48</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="10">
-        <v>48</v>
-      </c>
       <c r="I5" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A6" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="10">
-        <f>MIN(B4, B5)*2</f>
-        <v>96</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="B6" s="49">
+        <f>B4*1.5</f>
+        <v>105</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="49">
         <f>MIN(E4, E5)*2</f>
         <v>96</v>
       </c>
-      <c r="F6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="10">
-        <f>MIN(H4, H5)*2</f>
-        <v>96</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="44" t="s">
+      <c r="F6" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B7" s="45"/>
+      <c r="E7" s="45"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="45">
+        <v>0</v>
+      </c>
+      <c r="E8" s="45">
+        <v>0</v>
+      </c>
+      <c r="N8" s="50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="45">
+        <v>3</v>
+      </c>
+      <c r="E9" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E10" s="45">
         <v>1</v>
       </c>
-      <c r="H8" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="10">
-        <v>3</v>
-      </c>
-      <c r="E9" s="10">
-        <v>3</v>
-      </c>
-      <c r="H9" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="44" t="s">
+      <c r="N10" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="O10" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="P10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" s="51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="N11" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="O11" s="51">
+        <f>B2/B3*3</f>
+        <v>210</v>
+      </c>
+      <c r="P11" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="51">
+        <f>O11</f>
+        <v>210</v>
+      </c>
+      <c r="R11" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A12" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="45">
         <f>B6*B3</f>
-        <v>864</v>
+        <v>945</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="45">
         <f>E6*E3</f>
         <v>864</v>
       </c>
       <c r="F12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="10">
-        <f>H6*H3</f>
+      <c r="N12" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="O12" s="51">
+        <v>0</v>
+      </c>
+      <c r="P12" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="51">
+        <f>Q11</f>
+        <v>210</v>
+      </c>
+      <c r="R12" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S12" s="51"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="45">
+        <f>B12*B8</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="45">
+        <f>E12*E8</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="51">
+        <f>1.5*O11</f>
+        <v>315</v>
+      </c>
+      <c r="P13" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="51">
+        <f>1.5*(Q11+Q12)</f>
+        <v>630</v>
+      </c>
+      <c r="R13" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A14" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="46">
+        <f>B12+B13</f>
+        <v>945</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="46">
+        <f>E12+E13</f>
         <v>864</v>
       </c>
-      <c r="I12" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A13" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="10">
-        <f>B12*B8</f>
-        <v>864</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="10">
-        <f>E12*E8</f>
-        <v>864</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="10">
-        <f>H12*H8</f>
-        <v>864</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A14" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="43">
-        <f>B12+B13</f>
-        <v>1728</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="43">
-        <f>E12+E13</f>
-        <v>1728</v>
-      </c>
       <c r="F14" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="43">
-        <f>H12+H13</f>
-        <v>1728</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A16" s="44" t="s">
+      <c r="N14" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="51">
+        <f>4*3</f>
+        <v>12</v>
+      </c>
+      <c r="P14" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="51">
+        <f>4*6</f>
+        <v>24</v>
+      </c>
+      <c r="R14" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" s="51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="N15" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="51">
+        <v>2</v>
+      </c>
+      <c r="P15" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>2</v>
+      </c>
+      <c r="R15" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A16" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="45">
         <f>B2/B9/B10</f>
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="45">
         <f>E2/E9/E10</f>
-        <v>169.61490885416666</v>
+        <v>210</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="12">
-        <f>H2/H9/H10</f>
-        <v>171.17252604166666</v>
-      </c>
-      <c r="I16" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="44" t="s">
+      <c r="N16" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="O16" s="59">
+        <f>SUM(O11:O15)</f>
+        <v>539</v>
+      </c>
+      <c r="P16" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="59">
+        <f>SUM(Q11:Q15)</f>
+        <v>1076</v>
+      </c>
+      <c r="R16" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="S16" s="59" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="45">
         <f>B16*B8</f>
-        <v>259</v>
+        <v>0</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="45">
         <f>E16*E8</f>
-        <v>169.61490885416666</v>
+        <v>0</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="12">
-        <f>H16*H8</f>
-        <v>171.17252604166666</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="44" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="45">
         <f>B12/B9/B10</f>
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="C18" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="45">
         <f>E12/E9/E10</f>
         <v>288</v>
       </c>
       <c r="F18" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="12">
-        <f>H12/H9/H10</f>
-        <v>288</v>
-      </c>
-      <c r="I18" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="44" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="45">
         <f>B18*B8</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="45">
         <f>E18*E8</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="12">
-        <f>H18*H8</f>
-        <v>288</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="44" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="46">
         <f>SUM(B16:B19)</f>
-        <v>1094</v>
+        <v>525</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="46">
         <f>SUM(E16:E19)</f>
-        <v>915.22981770833326</v>
+        <v>498</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="45">
-        <f>SUM(H16:H19)</f>
-        <v>918.34505208333326</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="47">
-        <v>40806746</v>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="44">
+        <f>42063754</f>
+        <v>42063754</v>
+      </c>
+      <c r="E24" s="44">
+        <f>B24</f>
+        <v>42063754</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>